<commit_message>
Update Bloc 3 - Intro
</commit_message>
<xml_diff>
--- a/outils_numeriques/Grilles_Eval.xlsx
+++ b/outils_numeriques/Grilles_Eval.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tools\git_repo\semester-5\outils_numeriques\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tools\git_repo\digital_methods\semester-5\outils_numeriques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385E9B35-CBA5-475A-BF82-A4785574E5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBC926B-2CED-4CE8-B477-879FBE285488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="v2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>NOM</t>
   </si>
@@ -106,13 +107,43 @@
   </si>
   <si>
     <t>Bloc 1</t>
+  </si>
+  <si>
+    <t>S'APPROPRIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMS : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gpe : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ONIP / Outils Numériques pour l'Ingénieur.e en Physique </t>
+  </si>
+  <si>
+    <t>BLOC 1</t>
+  </si>
+  <si>
+    <t>BLOC 2</t>
+  </si>
+  <si>
+    <t>BLOC 3</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Compréhension du sujet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +175,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -159,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -346,11 +385,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -376,6 +428,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -385,10 +443,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -676,8 +746,8 @@
   </sheetPr>
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A39" sqref="A8:XFD39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,60 +768,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
     </row>
     <row r="2" spans="1:24" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
     </row>
     <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -759,33 +829,33 @@
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="G4" s="19" t="s">
+      <c r="E4" s="22"/>
+      <c r="G4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="20"/>
-      <c r="K4" s="19" t="s">
+      <c r="H4" s="23"/>
+      <c r="I4" s="22"/>
+      <c r="K4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="20"/>
-      <c r="Q4" s="19" t="s">
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="22"/>
+      <c r="Q4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="21"/>
-      <c r="S4" s="20"/>
-      <c r="U4" s="19" t="s">
+      <c r="R4" s="23"/>
+      <c r="S4" s="22"/>
+      <c r="U4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="20"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="22"/>
     </row>
     <row r="5" spans="1:24" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:24" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1723,4 +1793,139 @@
   <pageMargins left="0.27559055118110237" right="0.27559055118110237" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B408A4-E18F-4ACC-B8E2-C33B24138201}">
+  <dimension ref="A1:Q9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="43.44140625" customWidth="1"/>
+    <col min="3" max="3" width="1.6640625" customWidth="1"/>
+    <col min="4" max="7" width="2.77734375" customWidth="1"/>
+    <col min="8" max="8" width="1.6640625" customWidth="1"/>
+    <col min="9" max="12" width="2.77734375" customWidth="1"/>
+    <col min="13" max="13" width="1.6640625" customWidth="1"/>
+    <col min="14" max="17" width="2.77734375" customWidth="1"/>
+    <col min="18" max="18" width="1.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="26"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="D4" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D5" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
+      <c r="I5" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="30"/>
+      <c r="N5" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="N5:Q5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>